<commit_message>
1. Contribute pages. 2. Update map JSON with the updated information from Google sheet. 3. Add Media Center block to News and Blog main page.
</commit_message>
<xml_diff>
--- a/assets/js/map/PWNA MAP Information.xlsx
+++ b/assets/js/map/PWNA MAP Information.xlsx
@@ -10,8 +10,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="I1">
+      <text>
+        <t xml:space="preserve">Applied number format
+	-Alicia Searfoss</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D1">
+      <text>
+        <t xml:space="preserve">Applied number format
+	-Alicia Searfoss</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="256">
   <si>
     <t>Service Area</t>
   </si>
@@ -61,7 +83,7 @@
     <t>MT</t>
   </si>
   <si>
-    <t>45.347810, -100.40613</t>
+    <t>48.666644, -112.917583</t>
   </si>
   <si>
     <t>Babb, Browning, Heart Butte, Sevill</t>
@@ -91,7 +113,7 @@
     <t>SD</t>
   </si>
   <si>
-    <t>44.056263, -99.322921</t>
+    <t>44.166655,-99.45872</t>
   </si>
   <si>
     <t>Big Bend, Decker, Ft. Thompson, Stephen</t>
@@ -143,7 +165,7 @@
     <t>Salish-Kootenai Tribes</t>
   </si>
   <si>
-    <t>48.023689, -113.807820</t>
+    <t>47.50022, -114.334291</t>
   </si>
   <si>
     <t>Elmo, Hot Springs, Pablo, Polson, Ronan, St. Ignatius</t>
@@ -267,7 +289,7 @@
     <t>Santee Sioux Tribe</t>
   </si>
   <si>
-    <t>42.839310, -97.849229</t>
+    <t>42,713113, -97.828637</t>
   </si>
   <si>
     <t>Niobrara, Santee</t>
@@ -279,7 +301,7 @@
     <t>Lake Traverse/Sisseton-Wahpeton Tribe</t>
   </si>
   <si>
-    <t>45.652347, -97.060255</t>
+    <t>45.611639, -97.033577</t>
   </si>
   <si>
     <t>Agency Village, Enemy Swim, New Effington, Peever, Sisseton, Veblen, Waubay, Summit</t>
@@ -306,7 +328,7 @@
     <t>Standing Rock</t>
   </si>
   <si>
-    <t>46.065735, -100.634859</t>
+    <t>45.750275, -101.200415</t>
   </si>
   <si>
     <t>ND-Cannonball, Ft. Yates, Porcupine, Selfridge, Solen</t>
@@ -357,7 +379,7 @@
     <t>Yankton Sioux</t>
   </si>
   <si>
-    <t>43.039376, -98.184870</t>
+    <t>43.083327, -98.383691</t>
   </si>
   <si>
     <t>Lake Andes, Marty, Wagner</t>
@@ -378,7 +400,7 @@
     <t>UT</t>
   </si>
   <si>
-    <t>37.034162, -110.869586</t>
+    <t>37.034162, -110869586</t>
   </si>
   <si>
     <t>Aneth, Blanding, Bluff, Montezuma, Creek, Monument Valley</t>
@@ -393,7 +415,7 @@
     <t>NM</t>
   </si>
   <si>
-    <t>36.067217, -109.188005</t>
+    <t>36.067217, -108.188005</t>
   </si>
   <si>
     <t>Alamo, Becenti, Beclabito, Belen, Bloomfield, Breadsprings, Brimhall, Burnham, Cameron, Canoncito, Church Rock, Counselor, Coyote Canyon, Crownpoint, Cuba, Daltons Pass (Nahodishgish), Farmington, Forest Lake, Fruitland, Ft. Wingate, Gallup, Gamerco, Hogback, Iyanbito, Laguna, Lake Valley, Manuelito, Mariano Lake, Mentmore, Mexican Springs, Milan, Nageezi, Nenahnezad, Naschitti, Navajo, Newcomb, Ojo Encino, Pinedale, Pine Hill, Prewitt, Pueblo Pintado, Ramah, Red Rock, Rock Springs, Sanostee, Sheep Springs, Shiprock, Smith Lake, Standing Rock, Thoreau, To'hajiilee, Tohatchi, Torreon, Twin Lakes, Two Grey Hills, Upper Fruitland, Vanderwagen, White Rock, Whitehorse Lake, Window Rock, Ya-Ta-Hey
@@ -406,11 +428,14 @@
     <t>AZ, NM, UT</t>
   </si>
   <si>
+    <t>36.067217, -109.188005</t>
+  </si>
+  <si>
     <t>Blue Gap, Chambers, Chilchinbito, Chinle, Cornfields, Cottonwood, Cove, Dennehotso, Dilkon, Forest Lake, Ft. Defiance, Ganado, Greasewood, Hard Rock, Holbrook, Houck, Indian Wells, Inscription House, Kaibeto, Kayenta, Keams Canyon, Leupp, Low Mountain, Lukachukai, Lupton, Many Farms, Mitten Rock, Navajo Mountain, Nazlini, Page, Pinon, Red Lake, Red Valley, Rock Point, Rough Rock, Round Rock, Sanders, Sawmill, Shonto, St. Michaels, Steamboat, Sweetwater, Teec Nos Pos, Teesto, Tonalea, Tsaile, Tuba City, Whippoorwill Springs, White Cone, Window Rock and Winslow
 </t>
   </si>
   <si>
-    <t>11601856 (101835-AZ, 65764-NM, 6068-UT)</t>
+    <t>11,601,856 (101835-AZ, 65764-NM, 6068-UT)</t>
   </si>
   <si>
     <t>Acoma Indian Reservation</t>
@@ -419,13 +444,13 @@
     <t>Acoma Pueblo</t>
   </si>
   <si>
-    <t>35.523240, -109.854660</t>
+    <t>34.896319, -107.582309</t>
   </si>
   <si>
     <t>Pueblo of Acoma, Acomita</t>
   </si>
   <si>
-    <t>Ak-Chin Reservation</t>
+    <t>Ak-Chin (Maricopa) Reservation</t>
   </si>
   <si>
     <t>Ak-Chin</t>
@@ -557,7 +582,7 @@
     <t>Isleto Pueblo</t>
   </si>
   <si>
-    <t>37.199594, -107.858505</t>
+    <t>34.906996, -106.680859</t>
   </si>
   <si>
     <t>Jemez Indian Reservation</t>
@@ -566,7 +591,7 @@
     <t>Jemez Pueblo</t>
   </si>
   <si>
-    <t>36.012416, -106.058409</t>
+    <t>35.613917, -106.725868</t>
   </si>
   <si>
     <t>Jicarilla Apache Indian Reservation</t>
@@ -575,7 +600,7 @@
     <t>Jicarilla Apache</t>
   </si>
   <si>
-    <t>36.659077, -107.006703</t>
+    <t>32.956476, -105.650733</t>
   </si>
   <si>
     <t>Dulce</t>
@@ -587,7 +612,7 @@
     <t>Laguna</t>
   </si>
   <si>
-    <t>32.912827, -116.478072</t>
+    <t>35.036711, -107.382823</t>
   </si>
   <si>
     <t>Mescalero Indian Reservation</t>
@@ -605,7 +630,7 @@
     <t>Pojoaque Pueblo</t>
   </si>
   <si>
-    <t>34.519940, -105.870090</t>
+    <t>35.3892803, -106.023078</t>
   </si>
   <si>
     <t>Santa Fe</t>
@@ -647,7 +672,7 @@
     <t>San Carlos Apache</t>
   </si>
   <si>
-    <t>33.383388, -110.100647</t>
+    <t>33.345335, -110.453155</t>
   </si>
   <si>
     <t>San Carlos, Bylas</t>
@@ -656,7 +681,7 @@
     <t>San Felipe</t>
   </si>
   <si>
-    <t>35.415223, -106.400606</t>
+    <t>35.433925, -106.446693</t>
   </si>
   <si>
     <t>Bernalillo</t>
@@ -668,7 +693,7 @@
     <t>San Ildefonse</t>
   </si>
   <si>
-    <t>36.005920, -106.050798</t>
+    <t>35.891969, -106.118358</t>
   </si>
   <si>
     <t>San Juan Pueblo Indian Reservation</t>
@@ -689,7 +714,7 @@
     <t>San Dia</t>
   </si>
   <si>
-    <t>35.988216, -106.064566</t>
+    <t>32.309829, -104.83246</t>
   </si>
   <si>
     <t>Santa Ana Indian Reservation</t>
@@ -698,7 +723,7 @@
     <t>Santa Ana</t>
   </si>
   <si>
-    <t>33.794021, -116.504411</t>
+    <t>35.469294, -106.613731</t>
   </si>
   <si>
     <t>Santa Clara Indian Reservation</t>
@@ -707,7 +732,7 @@
     <t>Santa Clara Pueblo</t>
   </si>
   <si>
-    <t>36.010852, -106.116077</t>
+    <t>35.976573, -106.181145</t>
   </si>
   <si>
     <t>Espanola</t>
@@ -719,7 +744,7 @@
     <t>Santa Domingo (Kewa Pueblo)</t>
   </si>
   <si>
-    <t>35.519756, -106.370026</t>
+    <t>35.518490, -106.371346</t>
   </si>
   <si>
     <t>Kewa Pueblo (Formerly Santo Domingo)</t>
@@ -731,7 +756,7 @@
     <t>Tonto Apache</t>
   </si>
   <si>
-    <t>33.840641, -116.482713</t>
+    <t>36.422299, -105.597796</t>
   </si>
   <si>
     <t>Taos</t>
@@ -743,7 +768,7 @@
     <t>Pueblo of Tesuque</t>
   </si>
   <si>
-    <t>36.004749, -106.047181</t>
+    <t>35.806547, -105.973349</t>
   </si>
   <si>
     <t>Tohono O'Odham Indian Reservation</t>
@@ -764,7 +789,7 @@
     <t>Yavapai-Prescott</t>
   </si>
   <si>
-    <t>34.537928, -112.48311</t>
+    <t>34.53715, -112.452621</t>
   </si>
   <si>
     <t>Camp Verde, Prescott</t>
@@ -776,7 +801,7 @@
     <t>Zuni Pueblo</t>
   </si>
   <si>
-    <t>35.047136, -108.712579</t>
+    <t>35.044653, -108.711433</t>
   </si>
   <si>
     <t>Zuni</t>
@@ -786,8 +811,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00&quot;$&quot;"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0_);(#,##0)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot;$&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -819,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -830,16 +856,26 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -938,10 +974,10 @@
       <c r="H2" s="5">
         <v>0.395</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="6">
         <v>16000.0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="7">
         <v>1010472.63</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -973,10 +1009,10 @@
       <c r="H3" s="3">
         <v>28.3</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="6">
         <v>11357.0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="7">
         <v>1536317.84</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1008,10 +1044,10 @@
       <c r="H4" s="3">
         <v>40.3</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="6">
         <v>3429.0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="8">
         <v>151512.0</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1043,10 +1079,10 @@
       <c r="H5" s="3">
         <v>36.4</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="6">
         <v>15993.0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="7">
         <v>1.448855613E7</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1075,13 +1111,13 @@
       <c r="G6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="9">
         <v>0.18</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="6">
         <v>5675.0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="7">
         <v>522671.07</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1113,10 +1149,10 @@
       <c r="H7" s="5">
         <v>0.394</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="6">
         <v>6693.0</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="7">
         <v>619035.71</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1148,10 +1184,10 @@
       <c r="H8" s="5">
         <v>0.238</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="6">
         <v>7753.0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="7">
         <v>817631.56</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1183,10 +1219,10 @@
       <c r="H9" s="5">
         <v>0.296</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="6">
         <v>11786.0</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="7">
         <v>937046.28</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -1203,7 +1239,7 @@
       <c r="C10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>418.0</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1218,10 +1254,10 @@
       <c r="H10" s="5">
         <v>0.128</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="6">
         <v>423.0</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="8">
         <v>2184.0</v>
       </c>
       <c r="L10" s="3" t="s">
@@ -1253,10 +1289,10 @@
       <c r="H11" s="5">
         <v>0.322</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="6">
         <v>3410.0</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="7">
         <v>144587.96</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -1288,10 +1324,10 @@
       <c r="H12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="6">
         <v>10500.0</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="7">
         <v>440882.43</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -1323,10 +1359,10 @@
       <c r="H13" s="5">
         <v>0.254</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="6">
         <v>5427.0</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="7">
         <v>26911.5</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -1343,7 +1379,7 @@
       <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>10.0</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1355,13 +1391,13 @@
       <c r="G14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="9">
         <v>0.0</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="6">
         <v>2800.0</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="7">
         <v>725.85</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -1390,13 +1426,13 @@
       <c r="G15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="9">
         <v>0.49</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="6">
         <v>46885.0</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="7">
         <v>1775412.72</v>
       </c>
       <c r="L15" s="3" t="s">
@@ -1428,10 +1464,10 @@
       <c r="H16" s="3">
         <v>36.3</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="6">
         <v>6177.0</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="7">
         <v>110950.2</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -1463,10 +1499,10 @@
       <c r="H17" s="5">
         <v>0.467</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="6">
         <v>24217.0</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="7">
         <v>884194.01</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -1483,7 +1519,7 @@
       <c r="C18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="4">
         <v>901.0</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1498,10 +1534,10 @@
       <c r="H18" s="5">
         <v>0.337</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="6">
         <v>2662.0</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="7">
         <v>10198.06</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -1518,7 +1554,7 @@
       <c r="C19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="4">
         <v>10922.0</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1533,9 +1569,10 @@
       <c r="H19" s="5">
         <v>0.222</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="6">
         <v>12925.0</v>
       </c>
+      <c r="J19" s="10"/>
       <c r="L19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1562,13 +1599,13 @@
       <c r="G20" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="9">
         <v>0.48</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="6">
         <v>6748.0</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="7">
         <v>67821.87</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -1600,10 +1637,10 @@
       <c r="H21" s="5">
         <v>0.423</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="6">
         <v>16000.0</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="7">
         <v>840911.21</v>
       </c>
       <c r="L21" s="3" t="s">
@@ -1635,10 +1672,10 @@
       <c r="H22" s="5">
         <v>0.398</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="6">
         <v>30995.0</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="7">
         <v>77619.21</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -1670,10 +1707,10 @@
       <c r="H23" s="5">
         <v>0.251</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="6">
         <v>4192.0</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="7">
         <v>28167.08</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -1705,10 +1742,10 @@
       <c r="H24" s="5">
         <v>0.175</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="6">
         <v>11141.0</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="7">
         <v>1889708.19</v>
       </c>
       <c r="L24" s="3" t="s">
@@ -1740,10 +1777,10 @@
       <c r="H25" s="3">
         <v>30.45</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="6">
         <v>8300.0</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="7">
         <v>36740.97</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -1760,7 +1797,7 @@
       <c r="C26" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1775,10 +1812,10 @@
       <c r="H26" s="5">
         <v>0.413</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="8">
         <v>1234107.0</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -1795,7 +1832,7 @@
       <c r="C27" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1810,10 +1847,10 @@
       <c r="H27" s="5">
         <v>0.413</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="8">
         <v>4192063.0</v>
       </c>
       <c r="L27" s="3" t="s">
@@ -1837,19 +1874,19 @@
         <v>129</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H28" s="5">
         <v>0.413</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="6">
         <v>300048.0</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>123</v>
@@ -1860,10 +1897,10 @@
         <v>116</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D29" s="4">
         <v>3011.0</v>
@@ -1872,18 +1909,18 @@
         <v>125</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H29" s="5">
         <v>0.316</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="6">
         <v>6344.0</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="8">
         <v>378262.0</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -1895,30 +1932,30 @@
         <v>116</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D30" s="4">
         <v>1001.0</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H30" s="3">
         <v>47.5</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="6">
         <v>770.0</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="8">
         <v>21840.0</v>
       </c>
       <c r="L30" s="3" t="s">
@@ -1930,30 +1967,30 @@
         <v>116</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="3">
+        <v>143</v>
+      </c>
+      <c r="D31" s="4">
         <v>308.0</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H31" s="5">
         <v>0.353</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="6">
         <v>700.0</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="8">
         <v>30653.0</v>
       </c>
       <c r="L31" s="3" t="s">
@@ -1965,30 +2002,30 @@
         <v>116</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D32" s="3">
+        <v>148</v>
+      </c>
+      <c r="D32" s="4">
         <v>963.0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H32" s="5">
         <v>0.348</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="6">
         <v>1000.0</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="8">
         <v>6500.0</v>
       </c>
       <c r="L32" s="3" t="s">
@@ -2000,30 +2037,30 @@
         <v>116</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D33" s="4">
         <v>8764.0</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H33" s="5">
         <v>0.228</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="6">
         <v>3786.0</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="8">
         <v>269921.0</v>
       </c>
       <c r="L33" s="3" t="s">
@@ -2035,30 +2072,30 @@
         <v>116</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D34" s="4">
         <v>13409.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H34" s="5">
         <v>0.484</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="6">
         <v>15000.0</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="8">
         <v>1684226.0</v>
       </c>
       <c r="L34" s="3" t="s">
@@ -2070,30 +2107,30 @@
         <v>116</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D35" s="4">
         <v>2197.0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H35" s="5">
         <v>0.352</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="6">
         <v>2475.0</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="8">
         <v>43961.0</v>
       </c>
       <c r="L35" s="3" t="s">
@@ -2105,30 +2142,30 @@
         <v>116</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D36" s="4">
         <v>11712.0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H36" s="5">
         <v>0.521</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="6">
         <v>21502.0</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="8">
         <v>371823.0</v>
       </c>
       <c r="L36" s="3" t="s">
@@ -2140,30 +2177,30 @@
         <v>116</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D37" s="3">
+        <v>168</v>
+      </c>
+      <c r="D37" s="4">
         <v>465.0</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H37" s="5">
         <v>0.309</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="6">
         <v>674.0</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="8">
         <v>188077.0</v>
       </c>
       <c r="L37" s="3" t="s">
@@ -2175,30 +2212,30 @@
         <v>116</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D38" s="4">
         <v>7185.0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H38" s="5">
         <v>0.318</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="6">
         <v>18327.0</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="8">
         <v>1621044.0</v>
       </c>
       <c r="L38" s="3" t="s">
@@ -2210,30 +2247,30 @@
         <v>116</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D39" s="4">
         <v>1335.0</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H39" s="5">
         <v>0.351</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="6">
         <v>2300.0</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="8">
         <v>992463.0</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -2245,10 +2282,10 @@
         <v>116</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D40" s="4">
         <v>3400.0</v>
@@ -2257,18 +2294,18 @@
         <v>125</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="H40" s="5">
         <v>0.223</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="6">
         <v>4441.0</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="8">
         <v>301103.0</v>
       </c>
       <c r="L40" s="3" t="s">
@@ -2280,10 +2317,10 @@
         <v>116</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D41" s="4">
         <v>1815.0</v>
@@ -2292,18 +2329,18 @@
         <v>125</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="H41" s="5">
         <v>0.204</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="6">
         <v>3486.0</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="8">
         <v>89619.0</v>
       </c>
       <c r="L41" s="3" t="s">
@@ -2315,10 +2352,10 @@
         <v>116</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D42" s="4">
         <v>3254.0</v>
@@ -2327,18 +2364,18 @@
         <v>125</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H42" s="5">
         <v>0.217</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="6">
         <v>3403.0</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="8">
         <v>879917.0</v>
       </c>
       <c r="L42" s="3" t="s">
@@ -2350,10 +2387,10 @@
         <v>116</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D43" s="4">
         <v>4043.0</v>
@@ -2362,18 +2399,18 @@
         <v>125</v>
       </c>
       <c r="F43" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="H43" s="5">
         <v>0.362</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="6">
         <v>7825.0</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="8">
         <v>495423.0</v>
       </c>
       <c r="L43" s="3" t="s">
@@ -2385,10 +2422,10 @@
         <v>116</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D44" s="4">
         <v>3613.0</v>
@@ -2397,18 +2434,18 @@
         <v>125</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="H44" s="5">
         <v>0.422</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="6">
         <v>3979.0</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="8">
         <v>460769.0</v>
       </c>
       <c r="L44" s="3" t="s">
@@ -2420,10 +2457,10 @@
         <v>116</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D45" s="4">
         <v>3316.0</v>
@@ -2432,18 +2469,18 @@
         <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H45" s="5">
         <v>0.155</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="6">
         <v>327.0</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="8">
         <v>12004.0</v>
       </c>
       <c r="L45" s="3" t="s">
@@ -2455,10 +2492,10 @@
         <v>116</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D46" s="4">
         <v>1886.0</v>
@@ -2467,18 +2504,18 @@
         <v>125</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H46" s="5">
         <v>0.207</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="6">
         <v>324.0</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="8">
         <v>15034.0</v>
       </c>
       <c r="L46" s="3" t="s">
@@ -2490,10 +2527,10 @@
         <v>116</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D47" s="4">
         <v>1727.0</v>
@@ -2502,18 +2539,18 @@
         <v>125</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H47" s="5">
         <v>0.185</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="6">
         <v>1189.0</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="8">
         <v>50681.0</v>
       </c>
       <c r="L47" s="3" t="s">
@@ -2525,10 +2562,10 @@
         <v>116</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D48" s="4">
         <v>1611.0</v>
@@ -2537,18 +2574,18 @@
         <v>125</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H48" s="5">
         <v>0.117</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="6">
         <v>634.0</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="8">
         <v>19094.0</v>
       </c>
       <c r="L48" s="3" t="s">
@@ -2560,30 +2597,30 @@
         <v>116</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D49" s="4">
         <v>10068.0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="H49" s="6">
+        <v>212</v>
+      </c>
+      <c r="H49" s="9">
         <v>0.51</v>
       </c>
-      <c r="I49" s="4">
+      <c r="I49" s="6">
         <v>8921.0</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="8">
         <v>1822074.0</v>
       </c>
       <c r="L49" s="3" t="s">
@@ -2595,10 +2632,10 @@
         <v>116</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D50" s="4">
         <v>3185.0</v>
@@ -2607,18 +2644,18 @@
         <v>125</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H50" s="5">
         <v>0.303</v>
       </c>
-      <c r="I50" s="4">
+      <c r="I50" s="6">
         <v>3131.0</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="8">
         <v>48930.0</v>
       </c>
       <c r="L50" s="3" t="s">
@@ -2630,10 +2667,10 @@
         <v>116</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D51" s="4">
         <v>1752.0</v>
@@ -2642,18 +2679,18 @@
         <v>125</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H51" s="5">
         <v>0.131</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="6">
         <v>628.0</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="8">
         <v>28180.0</v>
       </c>
       <c r="L51" s="3" t="s">
@@ -2665,10 +2702,10 @@
         <v>116</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D52" s="4">
         <v>2668.0</v>
@@ -2677,15 +2714,15 @@
         <v>125</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="I52" s="3">
+        <v>222</v>
+      </c>
+      <c r="I52" s="6">
         <v>2723.0</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="8">
         <v>12236.0</v>
       </c>
       <c r="L52" s="3" t="s">
@@ -2697,30 +2734,30 @@
         <v>116</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D53" s="3">
+        <v>224</v>
+      </c>
+      <c r="D53" s="4">
         <v>4965.0</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H53" s="5">
         <v>0.268</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="6">
         <v>485.0</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="8">
         <v>22890.0</v>
       </c>
       <c r="L53" s="3" t="s">
@@ -2732,30 +2769,30 @@
         <v>116</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D54" s="3">
+        <v>227</v>
+      </c>
+      <c r="D54" s="4">
         <v>621.0</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H54" s="5">
         <v>0.139</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="6">
         <v>716.0</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="8">
         <v>77035.0</v>
       </c>
       <c r="L54" s="3" t="s">
@@ -2767,10 +2804,10 @@
         <v>116</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D55" s="4">
         <v>11021.0</v>
@@ -2779,18 +2816,18 @@
         <v>125</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H55" s="5">
         <v>0.235</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55" s="6">
         <v>2800.0</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="8">
         <v>53437.0</v>
       </c>
       <c r="L55" s="3" t="s">
@@ -2802,10 +2839,10 @@
         <v>116</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D56" s="4">
         <v>3255.0</v>
@@ -2814,18 +2851,18 @@
         <v>125</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H56" s="7">
+        <v>236</v>
+      </c>
+      <c r="H56" s="11">
         <v>32.9</v>
       </c>
-      <c r="I56" s="4">
+      <c r="I56" s="6">
         <v>4492.0</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="8">
         <v>71676.0</v>
       </c>
       <c r="L56" s="3" t="s">
@@ -2837,10 +2874,10 @@
         <v>116</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D57" s="4">
         <v>4384.0</v>
@@ -2849,18 +2886,18 @@
         <v>125</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H57" s="5">
         <v>0.189</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57" s="6">
         <v>2443.0</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="8">
         <v>96106.0</v>
       </c>
       <c r="L57" s="3" t="s">
@@ -2872,30 +2909,30 @@
         <v>116</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D58" s="3">
+        <v>242</v>
+      </c>
+      <c r="D58" s="4">
         <v>841.0</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H58" s="5">
         <v>0.192</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58" s="6">
         <v>404.0</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="8">
         <v>16813.0</v>
       </c>
       <c r="L58" s="3" t="s">
@@ -2907,30 +2944,30 @@
         <v>116</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D59" s="4">
         <v>10201.0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H59" s="5">
         <v>0.439</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I59" s="6">
         <v>27713.0</v>
       </c>
-      <c r="J59" s="4">
+      <c r="J59" s="8">
         <v>2846409.0</v>
       </c>
       <c r="L59" s="3" t="s">
@@ -2942,30 +2979,30 @@
         <v>116</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D60" s="3">
+        <v>249</v>
+      </c>
+      <c r="D60" s="4">
         <v>192.0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H60" s="5">
         <v>0.073</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="6">
         <v>159.0</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="8">
         <v>1403.0</v>
       </c>
       <c r="L60" s="3" t="s">
@@ -2977,10 +3014,10 @@
         <v>116</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D61" s="4">
         <v>7891.0</v>
@@ -2989,18 +3026,18 @@
         <v>125</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H61" s="5">
         <v>0.443</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="6">
         <v>9780.0</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="8">
         <v>463271.0</v>
       </c>
       <c r="L61" s="3" t="s">
@@ -3008,6 +3045,7 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Planned Giving sub-pages. 2. Map updates (BC) 3. Build sub-programs .LESS theme  configuration.
</commit_message>
<xml_diff>
--- a/assets/js/map/PWNA MAP Information.xlsx
+++ b/assets/js/map/PWNA MAP Information.xlsx
@@ -16,6 +16,14 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="F1">
+      <text>
+        <t xml:space="preserve">+rnassief@see3.com in the past I have separated X &amp; Y coordinates into different fields.   might want to consider that if doesnt cause more challenges.
+	-Mark Roth
+You are right. The API takes them separately and I do the split in the code.
+	-Romany Nassief</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="I1">
       <text>
         <t xml:space="preserve">Applied number format
@@ -33,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="313">
   <si>
     <t>Service Area</t>
   </si>
@@ -65,7 +73,7 @@
     <t>Size (acres)</t>
   </si>
   <si>
-    <t>Photo URL</t>
+    <t>Image</t>
   </si>
   <si>
     <t>Marker</t>
@@ -89,7 +97,10 @@
     <t>Babb, Browning, Heart Butte, Sevill</t>
   </si>
   <si>
-    <t>//nrcprograms.org/pwna_assets/images/marker_np.png</t>
+    <t>Blackfeet.jpg</t>
+  </si>
+  <si>
+    <t>marker_np.png</t>
   </si>
   <si>
     <t>Crow Agency Reservation</t>
@@ -104,6 +115,9 @@
     <t>Crow Agency, Ft. Smith, Lodge Grass, Pryor, St. Xavier, Wyola</t>
   </si>
   <si>
+    <t>CrowAgency.jpg</t>
+  </si>
+  <si>
     <t>Crow Creek Reservation</t>
   </si>
   <si>
@@ -117,6 +131,9 @@
   </si>
   <si>
     <t>Big Bend, Decker, Ft. Thompson, Stephen</t>
+  </si>
+  <si>
+    <t>CrowCreek.jpg</t>
   </si>
   <si>
     <t>Cheyenne River Reservation</t>
@@ -132,6 +149,9 @@
 </t>
   </si>
   <si>
+    <t>CheyenneRiver.jpg</t>
+  </si>
+  <si>
     <t>Fort Hall Reservation</t>
   </si>
   <si>
@@ -147,6 +167,9 @@
     <t>Fort Hall</t>
   </si>
   <si>
+    <t>FortHall.jpg</t>
+  </si>
+  <si>
     <t>Fort Belknap Reservation</t>
   </si>
   <si>
@@ -159,6 +182,9 @@
     <t>Dodson, Ft. Belknap Agency, Harlem, Hays, Lodge Pole</t>
   </si>
   <si>
+    <t>FortBelknap.jpg</t>
+  </si>
+  <si>
     <t>Flathead Nation Reservation</t>
   </si>
   <si>
@@ -171,6 +197,9 @@
     <t>Elmo, Hot Springs, Pablo, Polson, Ronan, St. Ignatius</t>
   </si>
   <si>
+    <t>Flathead.jpg</t>
+  </si>
+  <si>
     <t>Fort Peck Reservation</t>
   </si>
   <si>
@@ -183,6 +212,9 @@
     <t>Brockton, Frazer, Ft. Kipp, Poplar, Wolfpoint</t>
   </si>
   <si>
+    <t>FortPeck.jpg</t>
+  </si>
+  <si>
     <t>Flandreau Reservation</t>
   </si>
   <si>
@@ -195,6 +227,9 @@
     <t>Flandreau</t>
   </si>
   <si>
+    <t>Flandreau.gif</t>
+  </si>
+  <si>
     <t>Lower Brule Reservation</t>
   </si>
   <si>
@@ -207,6 +242,9 @@
     <t>Lower Brule</t>
   </si>
   <si>
+    <t>LowerBrule.jpg</t>
+  </si>
+  <si>
     <t>Northern Cheyenne Reservation</t>
   </si>
   <si>
@@ -222,6 +260,9 @@
     <t>36.4%/38.8%</t>
   </si>
   <si>
+    <t>NorthernCheyenne.jpg</t>
+  </si>
+  <si>
     <t>Omaha Reservation</t>
   </si>
   <si>
@@ -237,6 +278,9 @@
     <t>Macy, Walthill</t>
   </si>
   <si>
+    <t>Omaha.jpg</t>
+  </si>
+  <si>
     <t>Ponca Tribe of Nebraska</t>
   </si>
   <si>
@@ -247,6 +291,9 @@
   </si>
   <si>
     <t>Niobrara, Norfolk</t>
+  </si>
+  <si>
+    <t>Ponca.jpg</t>
   </si>
   <si>
     <t>Pine Ridge Reservation</t>
@@ -262,6 +309,9 @@
 </t>
   </si>
   <si>
+    <t>PineRidge.jpg</t>
+  </si>
+  <si>
     <t>Rocky Boy Reservation</t>
   </si>
   <si>
@@ -274,6 +324,9 @@
     <t>Box Elder, Rocky Boy</t>
   </si>
   <si>
+    <t>RockyBoy.jpg</t>
+  </si>
+  <si>
     <t>Rosebud Sioux Reservation</t>
   </si>
   <si>
@@ -283,18 +336,24 @@
     <t>43.187505, -100.625693</t>
   </si>
   <si>
+    <t>Rosebud.jpg</t>
+  </si>
+  <si>
     <t>Santee Sioux Reservation</t>
   </si>
   <si>
     <t>Santee Sioux Tribe</t>
   </si>
   <si>
-    <t>42,713113, -97.828637</t>
+    <t>42.839310, -97.849229</t>
   </si>
   <si>
     <t>Niobrara, Santee</t>
   </si>
   <si>
+    <t>Santee.gif</t>
+  </si>
+  <si>
     <t>Sisseton Wahpeton Oyate of the Lake Traverse Indian Reservation</t>
   </si>
   <si>
@@ -307,6 +366,9 @@
     <t>Agency Village, Enemy Swim, New Effington, Peever, Sisseton, Veblen, Waubay, Summit</t>
   </si>
   <si>
+    <t>SissetonLakeTraverse.jpg</t>
+  </si>
+  <si>
     <t>Spirit Lake Reservation</t>
   </si>
   <si>
@@ -322,6 +384,9 @@
     <t>Crow Hill, Fort Totten, Minnewaukan, St. Michael, Tokio, Warwick</t>
   </si>
   <si>
+    <t>SpiritLake.jpg</t>
+  </si>
+  <si>
     <t>Standing Rock Reservation</t>
   </si>
   <si>
@@ -334,6 +399,9 @@
     <t>ND-Cannonball, Ft. Yates, Porcupine, Selfridge, Solen</t>
   </si>
   <si>
+    <t>StandingRock.jpg</t>
+  </si>
+  <si>
     <t>Turtle Mountain Chippewa Reservation</t>
   </si>
   <si>
@@ -346,6 +414,9 @@
     <t>Belcourt, Dunseth, Rolla, St. John</t>
   </si>
   <si>
+    <t>TurtleMountain.jpg</t>
+  </si>
+  <si>
     <t>Winnebago Reservation</t>
   </si>
   <si>
@@ -358,6 +429,9 @@
     <t>Winnebago</t>
   </si>
   <si>
+    <t>Winnebago.jpg</t>
+  </si>
+  <si>
     <t>Wind River Reservation</t>
   </si>
   <si>
@@ -373,6 +447,9 @@
     <t>Arapahoe, St. Stephens, Crowheart, Ethete, Fort Washakie</t>
   </si>
   <si>
+    <t>WindRiver.jpg</t>
+  </si>
+  <si>
     <t>Yankton Sioux Reservation</t>
   </si>
   <si>
@@ -385,6 +462,9 @@
     <t>Lake Andes, Marty, Wagner</t>
   </si>
   <si>
+    <t>Yankton.jpg</t>
+  </si>
+  <si>
     <t>Southwest</t>
   </si>
   <si>
@@ -394,25 +474,31 @@
     <t>Navajo</t>
   </si>
   <si>
-    <t>See Below</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>37.034162, -110869586</t>
+    <t>173,667 (for entire Tribe)</t>
+  </si>
+  <si>
+    <t>AZ, NM, UT</t>
+  </si>
+  <si>
+    <t>37.034162, -110.869586</t>
   </si>
   <si>
     <t>Aneth, Blanding, Bluff, Montezuma, Creek, Monument Valley</t>
   </si>
   <si>
-    <t>//nrcprograms.org/pwna_assets/images/marker_sw.png</t>
-  </si>
-  <si>
-    <t>see below</t>
-  </si>
-  <si>
-    <t>NM</t>
+    <t>41.3%  (for entire Tribe)</t>
+  </si>
+  <si>
+    <t>300,048 (for entire Tribe)</t>
+  </si>
+  <si>
+    <t>11,601,856 (for Navajo Reservation as a whole)</t>
+  </si>
+  <si>
+    <t>Navajo.jpg</t>
+  </si>
+  <si>
+    <t>marker_sw.png</t>
   </si>
   <si>
     <t>36.067217, -108.188005</t>
@@ -422,12 +508,6 @@
 </t>
   </si>
   <si>
-    <t>See below</t>
-  </si>
-  <si>
-    <t>AZ, NM, UT</t>
-  </si>
-  <si>
     <t>36.067217, -109.188005</t>
   </si>
   <si>
@@ -435,21 +515,24 @@
 </t>
   </si>
   <si>
-    <t>11,601,856 (101835-AZ, 65764-NM, 6068-UT)</t>
-  </si>
-  <si>
     <t>Acoma Indian Reservation</t>
   </si>
   <si>
     <t>Acoma Pueblo</t>
   </si>
   <si>
+    <t>NM</t>
+  </si>
+  <si>
     <t>34.896319, -107.582309</t>
   </si>
   <si>
     <t>Pueblo of Acoma, Acomita</t>
   </si>
   <si>
+    <t>Acoma.jpg</t>
+  </si>
+  <si>
     <t>Ak-Chin (Maricopa) Reservation</t>
   </si>
   <si>
@@ -465,6 +548,9 @@
     <t>Maricopa, Stanfield</t>
   </si>
   <si>
+    <t>AkChin.gif</t>
+  </si>
+  <si>
     <t>Chemehuevi Indian Reservation</t>
   </si>
   <si>
@@ -480,6 +566,9 @@
     <t>Needles</t>
   </si>
   <si>
+    <t>Chemehuevi.gif</t>
+  </si>
+  <si>
     <t>Cocopah Indian Reservation</t>
   </si>
   <si>
@@ -492,6 +581,9 @@
     <t>Somerton</t>
   </si>
   <si>
+    <t>Cocopah.gif</t>
+  </si>
+  <si>
     <t>Colorado River Indian Reservation</t>
   </si>
   <si>
@@ -504,6 +596,9 @@
     <t>Parker</t>
   </si>
   <si>
+    <t>ColoradoRiver.gif</t>
+  </si>
+  <si>
     <t>Ft. Apache Indian Reservation</t>
   </si>
   <si>
@@ -516,6 +611,9 @@
     <t>Whiteriver, Cibecue, Pinetop, Show Low</t>
   </si>
   <si>
+    <t>FtApache.jpg</t>
+  </si>
+  <si>
     <t>Ft. Yuma Indian Reservation</t>
   </si>
   <si>
@@ -528,6 +626,9 @@
     <t>Yuma</t>
   </si>
   <si>
+    <t>FtYuma.jpg</t>
+  </si>
+  <si>
     <t>Gila River Indian Reservation</t>
   </si>
   <si>
@@ -540,6 +641,9 @@
     <t>Sacaton, Bapchule</t>
   </si>
   <si>
+    <t>GilaRiver.jpg</t>
+  </si>
+  <si>
     <t>Havasupai Indian Reservation</t>
   </si>
   <si>
@@ -552,6 +656,9 @@
     <t>Supai</t>
   </si>
   <si>
+    <t>Havasupai.gif</t>
+  </si>
+  <si>
     <t>Hopi Indian Reservation</t>
   </si>
   <si>
@@ -564,6 +671,9 @@
     <t>Sichomovi and Polacca (First Mesa); Mishongnovi and Sipaulovi (Second Mesa), Kykotsmovi Village, Hotevilla, and Moenkopi (Third Mesa)</t>
   </si>
   <si>
+    <t>Hopi.jpg</t>
+  </si>
+  <si>
     <t>Hualapai Indian Reservation</t>
   </si>
   <si>
@@ -576,6 +686,9 @@
     <t>Peach Springs</t>
   </si>
   <si>
+    <t>Hualapi.jpg</t>
+  </si>
+  <si>
     <t>Isleta Indian Reservation</t>
   </si>
   <si>
@@ -585,6 +698,9 @@
     <t>34.906996, -106.680859</t>
   </si>
   <si>
+    <t>Isleta.gif</t>
+  </si>
+  <si>
     <t>Jemez Indian Reservation</t>
   </si>
   <si>
@@ -594,6 +710,9 @@
     <t>35.613917, -106.725868</t>
   </si>
   <si>
+    <t>Jemez.jpg</t>
+  </si>
+  <si>
     <t>Jicarilla Apache Indian Reservation</t>
   </si>
   <si>
@@ -606,6 +725,9 @@
     <t>Dulce</t>
   </si>
   <si>
+    <t>Jicarilla.gif</t>
+  </si>
+  <si>
     <t>Laguna Indian Reservation</t>
   </si>
   <si>
@@ -615,6 +737,9 @@
     <t>35.036711, -107.382823</t>
   </si>
   <si>
+    <t>Laguna.jpg</t>
+  </si>
+  <si>
     <t>Mescalero Indian Reservation</t>
   </si>
   <si>
@@ -624,6 +749,9 @@
     <t>33.200088, -105.624152</t>
   </si>
   <si>
+    <t>Mescalero.gif</t>
+  </si>
+  <si>
     <t>Pojoaque Indian Reservation</t>
   </si>
   <si>
@@ -636,6 +764,9 @@
     <t>Santa Fe</t>
   </si>
   <si>
+    <t>Pojoaque.jpg</t>
+  </si>
+  <si>
     <t>Picuris Pueblo</t>
   </si>
   <si>
@@ -645,6 +776,9 @@
     <t>Penasco</t>
   </si>
   <si>
+    <t>Picuris.gif</t>
+  </si>
+  <si>
     <t>Pueblo of Cochiti</t>
   </si>
   <si>
@@ -657,6 +791,9 @@
     <t>Cochiti</t>
   </si>
   <si>
+    <t>Cochiti.gif</t>
+  </si>
+  <si>
     <t>Pueblo of Nambe</t>
   </si>
   <si>
@@ -666,6 +803,9 @@
     <t>35.885357, -105.959605</t>
   </si>
   <si>
+    <t>PuebloOfNambe.gif</t>
+  </si>
+  <si>
     <t>San Carlos Indian Reservation</t>
   </si>
   <si>
@@ -678,6 +818,9 @@
     <t>San Carlos, Bylas</t>
   </si>
   <si>
+    <t>SanCarlos.jpg</t>
+  </si>
+  <si>
     <t>San Felipe</t>
   </si>
   <si>
@@ -687,6 +830,9 @@
     <t>Bernalillo</t>
   </si>
   <si>
+    <t>SanFelipe.gif</t>
+  </si>
+  <si>
     <t>San Ildefonse Pueblo</t>
   </si>
   <si>
@@ -696,6 +842,9 @@
     <t>35.891969, -106.118358</t>
   </si>
   <si>
+    <t>SanIldefonso.gif</t>
+  </si>
+  <si>
     <t>San Juan Pueblo Indian Reservation</t>
   </si>
   <si>
@@ -708,6 +857,9 @@
     <t>Ohkay Owingeh (formerly San Juan Pueblo)</t>
   </si>
   <si>
+    <t>SanJuan.jpg</t>
+  </si>
+  <si>
     <t>Sandia Indian Reservation</t>
   </si>
   <si>
@@ -717,6 +869,9 @@
     <t>32.309829, -104.83246</t>
   </si>
   <si>
+    <t>Sandia.gif</t>
+  </si>
+  <si>
     <t>Santa Ana Indian Reservation</t>
   </si>
   <si>
@@ -726,6 +881,9 @@
     <t>35.469294, -106.613731</t>
   </si>
   <si>
+    <t>SantaAna.gif</t>
+  </si>
+  <si>
     <t>Santa Clara Indian Reservation</t>
   </si>
   <si>
@@ -738,6 +896,9 @@
     <t>Espanola</t>
   </si>
   <si>
+    <t>SC.jpg</t>
+  </si>
+  <si>
     <t>Santo Domingo Pueblo (Kewa Pueblo)</t>
   </si>
   <si>
@@ -750,6 +911,9 @@
     <t>Kewa Pueblo (Formerly Santo Domingo)</t>
   </si>
   <si>
+    <t>KewaPuebloSantoDomingo.jpg</t>
+  </si>
+  <si>
     <t>Taos Indian Reservation</t>
   </si>
   <si>
@@ -762,6 +926,9 @@
     <t>Taos</t>
   </si>
   <si>
+    <t>Taos.gif</t>
+  </si>
+  <si>
     <t>Tesuque Indian Reservation</t>
   </si>
   <si>
@@ -771,6 +938,9 @@
     <t>35.806547, -105.973349</t>
   </si>
   <si>
+    <t>Teseque.gif</t>
+  </si>
+  <si>
     <t>Tohono O'Odham Indian Reservation</t>
   </si>
   <si>
@@ -783,6 +953,9 @@
     <t>Sells, Ajo, Tucson, Hickewan, Pisenimo</t>
   </si>
   <si>
+    <t>Tohono.jpg</t>
+  </si>
+  <si>
     <t>Yavapai-Presecott Reservation</t>
   </si>
   <si>
@@ -795,6 +968,9 @@
     <t>Camp Verde, Prescott</t>
   </si>
   <si>
+    <t>Yavapai.gif</t>
+  </si>
+  <si>
     <t>Zuni Indian Reservation</t>
   </si>
   <si>
@@ -805,6 +981,9 @@
   </si>
   <si>
     <t>Zuni</t>
+  </si>
+  <si>
+    <t>Zuni.jpg</t>
   </si>
 </sst>
 </file>
@@ -874,7 +1053,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
@@ -893,9 +1074,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4.0" ySplit="2.0" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E1" sqref="E1" pane="topRight"/>
+      <selection activeCell="A3" sqref="A3" pane="bottomLeft"/>
+      <selection activeCell="E3" sqref="E3" pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="16.86"/>
+    <col customWidth="1" min="6" max="6" width="25.43"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -980,8 +1170,11 @@
       <c r="J2" s="7">
         <v>1010472.63</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="L2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -989,10 +1182,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4">
         <v>6863.0</v>
@@ -1001,10 +1194,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3">
         <v>28.3</v>
@@ -1015,8 +1208,11 @@
       <c r="J3" s="7">
         <v>1536317.84</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="L3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -1024,22 +1220,22 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4">
         <v>2010.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3">
         <v>40.3</v>
@@ -1050,8 +1246,11 @@
       <c r="J4" s="8">
         <v>151512.0</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -1059,22 +1258,22 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>8090.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3">
         <v>36.4</v>
@@ -1085,8 +1284,11 @@
       <c r="J5" s="7">
         <v>1.448855613E7</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -1094,22 +1296,22 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D6" s="4">
         <v>5767.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H6" s="9">
         <v>0.18</v>
@@ -1120,8 +1322,11 @@
       <c r="J6" s="7">
         <v>522671.07</v>
       </c>
+      <c r="K6" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -1129,10 +1334,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4">
         <v>2851.0</v>
@@ -1141,10 +1346,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H7" s="5">
         <v>0.394</v>
@@ -1155,8 +1360,11 @@
       <c r="J7" s="7">
         <v>619035.71</v>
       </c>
+      <c r="K7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="L7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -1164,10 +1372,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4">
         <v>28359.0</v>
@@ -1176,10 +1384,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H8" s="5">
         <v>0.238</v>
@@ -1190,8 +1398,11 @@
       <c r="J8" s="7">
         <v>817631.56</v>
       </c>
+      <c r="K8" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -1199,10 +1410,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D9" s="4">
         <v>10008.0</v>
@@ -1211,10 +1422,10 @@
         <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5">
         <v>0.296</v>
@@ -1225,8 +1436,11 @@
       <c r="J9" s="7">
         <v>937046.28</v>
       </c>
+      <c r="K9" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="L9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -1234,22 +1448,22 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D10" s="4">
         <v>418.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="H10" s="5">
         <v>0.128</v>
@@ -1260,8 +1474,11 @@
       <c r="J10" s="8">
         <v>2184.0</v>
       </c>
+      <c r="K10" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="L10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -1269,22 +1486,22 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D11" s="4">
         <v>1505.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H11" s="5">
         <v>0.322</v>
@@ -1295,8 +1512,11 @@
       <c r="J11" s="7">
         <v>144587.96</v>
       </c>
+      <c r="K11" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -1304,10 +1524,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D12" s="4">
         <v>4789.0</v>
@@ -1316,13 +1536,13 @@
         <v>15</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="I12" s="6">
         <v>10500.0</v>
@@ -1330,8 +1550,11 @@
       <c r="J12" s="7">
         <v>440882.43</v>
       </c>
+      <c r="K12" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="L12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -1339,22 +1562,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D13" s="4">
         <v>4773.0</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="H13" s="5">
         <v>0.254</v>
@@ -1365,8 +1588,11 @@
       <c r="J13" s="7">
         <v>26911.5</v>
       </c>
+      <c r="K13" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -1374,22 +1600,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4">
         <v>10.0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="H14" s="9">
         <v>0.0</v>
@@ -1400,8 +1626,11 @@
       <c r="J14" s="7">
         <v>725.85</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="L14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -1409,22 +1638,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D15" s="4">
         <v>18834.0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H15" s="9">
         <v>0.49</v>
@@ -1435,8 +1664,11 @@
       <c r="J15" s="7">
         <v>1775412.72</v>
       </c>
+      <c r="K15" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="L15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -1444,10 +1676,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D16" s="4">
         <v>3323.0</v>
@@ -1456,10 +1688,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="H16" s="3">
         <v>36.3</v>
@@ -1470,8 +1702,11 @@
       <c r="J16" s="7">
         <v>110950.2</v>
       </c>
+      <c r="K16" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="L16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -1479,22 +1714,22 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D17" s="4">
         <v>10869.0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H17" s="5">
         <v>0.467</v>
@@ -1505,8 +1740,11 @@
       <c r="J17" s="7">
         <v>884194.01</v>
       </c>
+      <c r="K17" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="L17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -1514,22 +1752,22 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D18" s="4">
         <v>901.0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="H18" s="5">
         <v>0.337</v>
@@ -1540,8 +1778,11 @@
       <c r="J18" s="7">
         <v>10198.06</v>
       </c>
+      <c r="K18" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="L18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
@@ -1549,22 +1790,22 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4">
         <v>10922.0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="H19" s="5">
         <v>0.222</v>
@@ -1572,9 +1813,14 @@
       <c r="I19" s="6">
         <v>12925.0</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="7">
+        <v>107902.7</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="L19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -1582,22 +1828,22 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D20" s="4">
         <v>4238.0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="H20" s="9">
         <v>0.48</v>
@@ -1608,8 +1854,11 @@
       <c r="J20" s="7">
         <v>67821.87</v>
       </c>
+      <c r="K20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="L20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -1617,22 +1866,22 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="D21" s="4">
         <v>8217.0</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="H21" s="5">
         <v>0.423</v>
@@ -1643,8 +1892,11 @@
       <c r="J21" s="7">
         <v>840911.21</v>
       </c>
+      <c r="K21" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="L21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -1652,22 +1904,22 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D22" s="4">
         <v>8669.0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="H22" s="5">
         <v>0.398</v>
@@ -1678,8 +1930,11 @@
       <c r="J22" s="7">
         <v>77619.21</v>
       </c>
+      <c r="K22" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -1687,22 +1942,22 @@
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D23" s="4">
         <v>2694.0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="H23" s="5">
         <v>0.251</v>
@@ -1713,8 +1968,11 @@
       <c r="J23" s="7">
         <v>28167.08</v>
       </c>
+      <c r="K23" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="L23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
@@ -1722,22 +1980,22 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D24" s="4">
         <v>26490.0</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="H24" s="5">
         <v>0.175</v>
@@ -1748,8 +2006,11 @@
       <c r="J24" s="7">
         <v>1889708.19</v>
       </c>
+      <c r="K24" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="L24" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
@@ -1757,22 +2018,22 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D25" s="4">
         <v>6465.0</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="H25" s="3">
         <v>30.45</v>
@@ -1783,136 +2044,148 @@
       <c r="J25" s="7">
         <v>36740.97</v>
       </c>
+      <c r="K25" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="L25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0.413</v>
+        <v>146</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J26" s="8">
-        <v>1234107.0</v>
+        <v>148</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0.413</v>
+        <v>153</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="J27" s="8">
-        <v>4192063.0</v>
+        <v>148</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="4">
-        <v>173667.0</v>
+        <v>142</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0.413</v>
-      </c>
-      <c r="I28" s="6">
-        <v>300048.0</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>132</v>
+        <v>155</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="D29" s="4">
         <v>3011.0</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="H29" s="5">
         <v>0.316</v>
@@ -1923,31 +2196,34 @@
       <c r="J29" s="8">
         <v>378262.0</v>
       </c>
+      <c r="K29" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="L29" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="D30" s="4">
         <v>1001.0</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="H30" s="3">
         <v>47.5</v>
@@ -1958,31 +2234,34 @@
       <c r="J30" s="8">
         <v>21840.0</v>
       </c>
+      <c r="K30" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="L30" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D31" s="4">
         <v>308.0</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="H31" s="5">
         <v>0.353</v>
@@ -1993,31 +2272,34 @@
       <c r="J31" s="8">
         <v>30653.0</v>
       </c>
+      <c r="K31" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="L31" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="D32" s="4">
         <v>963.0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="H32" s="5">
         <v>0.348</v>
@@ -2028,31 +2310,34 @@
       <c r="J32" s="8">
         <v>6500.0</v>
       </c>
+      <c r="K32" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="L32" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="D33" s="4">
         <v>8764.0</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="H33" s="5">
         <v>0.228</v>
@@ -2063,31 +2348,34 @@
       <c r="J33" s="8">
         <v>269921.0</v>
       </c>
+      <c r="K33" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="L33" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="D34" s="4">
         <v>13409.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="H34" s="5">
         <v>0.484</v>
@@ -2098,31 +2386,34 @@
       <c r="J34" s="8">
         <v>1684226.0</v>
       </c>
+      <c r="K34" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="L34" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="D35" s="4">
         <v>2197.0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="H35" s="5">
         <v>0.352</v>
@@ -2133,31 +2424,34 @@
       <c r="J35" s="8">
         <v>43961.0</v>
       </c>
+      <c r="K35" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="L35" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="D36" s="4">
         <v>11712.0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="H36" s="5">
         <v>0.521</v>
@@ -2168,31 +2462,34 @@
       <c r="J36" s="8">
         <v>371823.0</v>
       </c>
+      <c r="K36" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="L36" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="D37" s="4">
         <v>465.0</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="H37" s="5">
         <v>0.309</v>
@@ -2203,31 +2500,34 @@
       <c r="J37" s="8">
         <v>188077.0</v>
       </c>
+      <c r="K37" s="3" t="s">
+        <v>203</v>
+      </c>
       <c r="L37" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="D38" s="4">
         <v>7185.0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="H38" s="5">
         <v>0.318</v>
@@ -2238,31 +2538,34 @@
       <c r="J38" s="8">
         <v>1621044.0</v>
       </c>
+      <c r="K38" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="L38" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="D39" s="4">
         <v>1335.0</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="H39" s="5">
         <v>0.351</v>
@@ -2273,31 +2576,34 @@
       <c r="J39" s="8">
         <v>992463.0</v>
       </c>
+      <c r="K39" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="L39" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="D40" s="4">
         <v>3400.0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="H40" s="5">
         <v>0.223</v>
@@ -2308,31 +2614,34 @@
       <c r="J40" s="8">
         <v>301103.0</v>
       </c>
+      <c r="K40" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="L40" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="D41" s="4">
         <v>1815.0</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="H41" s="5">
         <v>0.204</v>
@@ -2343,31 +2652,34 @@
       <c r="J41" s="8">
         <v>89619.0</v>
       </c>
+      <c r="K41" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="L41" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="D42" s="4">
         <v>3254.0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="H42" s="5">
         <v>0.217</v>
@@ -2378,31 +2690,34 @@
       <c r="J42" s="8">
         <v>879917.0</v>
       </c>
+      <c r="K42" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="L42" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="D43" s="4">
         <v>4043.0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="H43" s="5">
         <v>0.362</v>
@@ -2413,31 +2728,34 @@
       <c r="J43" s="8">
         <v>495423.0</v>
       </c>
+      <c r="K43" s="3" t="s">
+        <v>230</v>
+      </c>
       <c r="L43" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="D44" s="4">
         <v>3613.0</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>194</v>
+        <v>233</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="H44" s="5">
         <v>0.422</v>
@@ -2448,31 +2766,34 @@
       <c r="J44" s="8">
         <v>460769.0</v>
       </c>
+      <c r="K44" s="3" t="s">
+        <v>234</v>
+      </c>
       <c r="L44" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="D45" s="4">
         <v>3316.0</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="H45" s="5">
         <v>0.155</v>
@@ -2483,31 +2804,34 @@
       <c r="J45" s="8">
         <v>12004.0</v>
       </c>
+      <c r="K45" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="L45" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="D46" s="4">
         <v>1886.0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="H46" s="5">
         <v>0.207</v>
@@ -2518,31 +2842,34 @@
       <c r="J46" s="8">
         <v>15034.0</v>
       </c>
+      <c r="K46" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="L46" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="D47" s="4">
         <v>1727.0</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="H47" s="5">
         <v>0.185</v>
@@ -2553,31 +2880,34 @@
       <c r="J47" s="8">
         <v>50681.0</v>
       </c>
+      <c r="K47" s="3" t="s">
+        <v>248</v>
+      </c>
       <c r="L47" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="D48" s="4">
         <v>1611.0</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="H48" s="5">
         <v>0.117</v>
@@ -2588,31 +2918,34 @@
       <c r="J48" s="8">
         <v>19094.0</v>
       </c>
+      <c r="K48" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="L48" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>209</v>
+        <v>253</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>210</v>
+        <v>254</v>
       </c>
       <c r="D49" s="4">
         <v>10068.0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>212</v>
+        <v>256</v>
       </c>
       <c r="H49" s="9">
         <v>0.51</v>
@@ -2623,31 +2956,34 @@
       <c r="J49" s="8">
         <v>1822074.0</v>
       </c>
+      <c r="K49" s="3" t="s">
+        <v>257</v>
+      </c>
       <c r="L49" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="D50" s="4">
         <v>3185.0</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="H50" s="5">
         <v>0.303</v>
@@ -2658,31 +2994,34 @@
       <c r="J50" s="8">
         <v>48930.0</v>
       </c>
+      <c r="K50" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="L50" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>216</v>
+        <v>262</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
       <c r="D51" s="4">
         <v>1752.0</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>218</v>
+        <v>264</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="H51" s="5">
         <v>0.131</v>
@@ -2693,31 +3032,34 @@
       <c r="J51" s="8">
         <v>28180.0</v>
       </c>
+      <c r="K51" s="3" t="s">
+        <v>265</v>
+      </c>
       <c r="L51" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>219</v>
+        <v>266</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>220</v>
+        <v>267</v>
       </c>
       <c r="D52" s="4">
         <v>2668.0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>221</v>
+        <v>268</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
       <c r="I52" s="6">
         <v>2723.0</v>
@@ -2725,31 +3067,34 @@
       <c r="J52" s="8">
         <v>12236.0</v>
       </c>
+      <c r="K52" s="3" t="s">
+        <v>270</v>
+      </c>
       <c r="L52" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="D53" s="4">
         <v>4965.0</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>225</v>
+        <v>273</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="H53" s="5">
         <v>0.268</v>
@@ -2760,31 +3105,34 @@
       <c r="J53" s="8">
         <v>22890.0</v>
       </c>
+      <c r="K53" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="L53" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>226</v>
+        <v>275</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>227</v>
+        <v>276</v>
       </c>
       <c r="D54" s="4">
         <v>621.0</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>228</v>
+        <v>277</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="H54" s="5">
         <v>0.139</v>
@@ -2795,31 +3143,34 @@
       <c r="J54" s="8">
         <v>77035.0</v>
       </c>
+      <c r="K54" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="L54" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="D55" s="4">
         <v>11021.0</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>231</v>
+        <v>281</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="H55" s="5">
         <v>0.235</v>
@@ -2830,31 +3181,34 @@
       <c r="J55" s="8">
         <v>53437.0</v>
       </c>
+      <c r="K55" s="3" t="s">
+        <v>283</v>
+      </c>
       <c r="L55" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
       <c r="D56" s="4">
         <v>3255.0</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>235</v>
+        <v>286</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>236</v>
+        <v>287</v>
       </c>
       <c r="H56" s="11">
         <v>32.9</v>
@@ -2865,31 +3219,34 @@
       <c r="J56" s="8">
         <v>71676.0</v>
       </c>
+      <c r="K56" s="3" t="s">
+        <v>288</v>
+      </c>
       <c r="L56" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>237</v>
+        <v>289</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>238</v>
+        <v>290</v>
       </c>
       <c r="D57" s="4">
         <v>4384.0</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>239</v>
+        <v>291</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>240</v>
+        <v>292</v>
       </c>
       <c r="H57" s="5">
         <v>0.189</v>
@@ -2900,31 +3257,34 @@
       <c r="J57" s="8">
         <v>96106.0</v>
       </c>
+      <c r="K57" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="L57" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>241</v>
+        <v>294</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="D58" s="4">
         <v>841.0</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>243</v>
+        <v>296</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="H58" s="5">
         <v>0.192</v>
@@ -2935,31 +3295,34 @@
       <c r="J58" s="8">
         <v>16813.0</v>
       </c>
+      <c r="K58" s="3" t="s">
+        <v>297</v>
+      </c>
       <c r="L58" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="D59" s="4">
         <v>10201.0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>246</v>
+        <v>300</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>247</v>
+        <v>301</v>
       </c>
       <c r="H59" s="5">
         <v>0.439</v>
@@ -2970,31 +3333,34 @@
       <c r="J59" s="8">
         <v>2846409.0</v>
       </c>
+      <c r="K59" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="L59" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>248</v>
+        <v>303</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>249</v>
+        <v>304</v>
       </c>
       <c r="D60" s="4">
         <v>192.0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>250</v>
+        <v>305</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>251</v>
+        <v>306</v>
       </c>
       <c r="H60" s="5">
         <v>0.073</v>
@@ -3005,31 +3371,34 @@
       <c r="J60" s="8">
         <v>1403.0</v>
       </c>
+      <c r="K60" s="3" t="s">
+        <v>307</v>
+      </c>
       <c r="L60" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>252</v>
+        <v>308</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>253</v>
+        <v>309</v>
       </c>
       <c r="D61" s="4">
         <v>7891.0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>254</v>
+        <v>310</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>255</v>
+        <v>311</v>
       </c>
       <c r="H61" s="5">
         <v>0.443</v>
@@ -3040,8 +3409,11 @@
       <c r="J61" s="8">
         <v>463271.0</v>
       </c>
+      <c r="K61" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="L61" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Homepage updates (red bar, slider indicator/caption, outcomes). 2. Working on punch list sheet. 3. First testing round
</commit_message>
<xml_diff>
--- a/assets/js/map/PWNA MAP Information.xlsx
+++ b/assets/js/map/PWNA MAP Information.xlsx
@@ -16,6 +16,14 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="K1">
+      <text>
+        <t xml:space="preserve">+lishsearfoss@gmail.com Link column added
+	-Romany Nassief
+Thanks, Rom!
+	-Alicia Searfoss</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F1">
       <text>
         <t xml:space="preserve">+rnassief@see3.com in the past I have separated X &amp; Y coordinates into different fields.   might want to consider that if doesnt cause more challenges.
@@ -41,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="318">
   <si>
     <t>Service Area</t>
   </si>
@@ -73,6 +81,9 @@
     <t>Size (acres)</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>Image</t>
   </si>
   <si>
@@ -97,6 +108,9 @@
     <t>Babb, Browning, Heart Butte, Sevill</t>
   </si>
   <si>
+    <t>PageServer?pagename=pwna&amp;page=airc_res_mt_blackfeet</t>
+  </si>
+  <si>
     <t>Blackfeet.jpg</t>
   </si>
   <si>
@@ -115,6 +129,9 @@
     <t>Crow Agency, Ft. Smith, Lodge Grass, Pryor, St. Xavier, Wyola</t>
   </si>
   <si>
+    <t>PageServer?pagename=pwna&amp;page=airc_res_mt_crow</t>
+  </si>
+  <si>
     <t>CrowAgency.jpg</t>
   </si>
   <si>
@@ -131,6 +148,9 @@
   </si>
   <si>
     <t>Big Bend, Decker, Ft. Thompson, Stephen</t>
+  </si>
+  <si>
+    <t>http://www.nrcprograms.org/site/PageServer?pagename=pwna&amp;page=airc_res_sd_crowcreek</t>
   </si>
   <si>
     <t>CrowCreek.jpg</t>
@@ -147,6 +167,9 @@
   <si>
     <t>Bridger, Cherry Creek, Dupree, Eagle Butte, Green Grass, Iron Lightning, Isabel,  La Plant,  Lantry, Red Scaffold, Ridgeview, Swift Bird, Takini, Thunder Butte, Timber Lake,  Whitehorse
 </t>
+  </si>
+  <si>
+    <t>http://www.nrcprograms.org/site/PageServer?pagename=pwna&amp;page=airc_res_sd_cheyenneriver</t>
   </si>
   <si>
     <t>CheyenneRiver.jpg</t>
@@ -994,7 +1017,7 @@
     <numFmt numFmtId="164" formatCode="#,##0_);(#,##0)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot;$&quot;"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1004,6 +1027,10 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1024,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1048,6 +1075,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1124,7 +1154,9 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -1138,28 +1170,29 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4">
         <v>10405.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="5">
         <v>0.395</v>
@@ -1171,33 +1204,36 @@
         <v>1010472.63</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4">
         <v>6863.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3">
         <v>28.3</v>
@@ -1209,33 +1245,36 @@
         <v>1536317.84</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>2010.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H4" s="3">
         <v>40.3</v>
@@ -1246,34 +1285,37 @@
       <c r="J4" s="8">
         <v>151512.0</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>30</v>
+      <c r="K4" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4">
         <v>8090.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H5" s="3">
         <v>36.4</v>
@@ -1284,36 +1326,39 @@
       <c r="J5" s="7">
         <v>1.448855613E7</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>35</v>
+      <c r="K5" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4">
         <v>5767.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="9">
+        <v>45</v>
+      </c>
+      <c r="H6" s="10">
         <v>0.18</v>
       </c>
       <c r="I6" s="6">
@@ -1322,34 +1367,35 @@
       <c r="J6" s="7">
         <v>522671.07</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>19</v>
+        <v>46</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4">
         <v>2851.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H7" s="5">
         <v>0.394</v>
@@ -1360,34 +1406,35 @@
       <c r="J7" s="7">
         <v>619035.71</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4">
         <v>28359.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5">
         <v>0.238</v>
@@ -1398,34 +1445,35 @@
       <c r="J8" s="7">
         <v>817631.56</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4">
         <v>10008.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5">
         <v>0.296</v>
@@ -1436,34 +1484,35 @@
       <c r="J9" s="7">
         <v>937046.28</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>19</v>
+        <v>61</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D10" s="4">
         <v>418.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H10" s="5">
         <v>0.128</v>
@@ -1474,34 +1523,35 @@
       <c r="J10" s="8">
         <v>2184.0</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>19</v>
+        <v>66</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D11" s="4">
         <v>1505.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H11" s="5">
         <v>0.322</v>
@@ -1512,37 +1562,38 @@
       <c r="J11" s="7">
         <v>144587.96</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4">
         <v>4789.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="I12" s="6">
         <v>10500.0</v>
@@ -1550,34 +1601,35 @@
       <c r="J12" s="7">
         <v>440882.43</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D13" s="4">
         <v>4773.0</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H13" s="5">
         <v>0.254</v>
@@ -1588,36 +1640,37 @@
       <c r="J13" s="7">
         <v>26911.5</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>19</v>
+        <v>83</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D14" s="4">
         <v>10.0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="9">
+        <v>87</v>
+      </c>
+      <c r="H14" s="10">
         <v>0.0</v>
       </c>
       <c r="I14" s="6">
@@ -1626,36 +1679,37 @@
       <c r="J14" s="7">
         <v>725.85</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D15" s="4">
         <v>18834.0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="9">
+        <v>92</v>
+      </c>
+      <c r="H15" s="10">
         <v>0.49</v>
       </c>
       <c r="I15" s="6">
@@ -1664,34 +1718,35 @@
       <c r="J15" s="7">
         <v>1775412.72</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>19</v>
+        <v>93</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D16" s="4">
         <v>3323.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H16" s="3">
         <v>36.3</v>
@@ -1702,34 +1757,35 @@
       <c r="J16" s="7">
         <v>110950.2</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>19</v>
+        <v>98</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D17" s="4">
         <v>10869.0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H17" s="5">
         <v>0.467</v>
@@ -1740,34 +1796,35 @@
       <c r="J17" s="7">
         <v>884194.01</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>102</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D18" s="4">
         <v>901.0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H18" s="5">
         <v>0.337</v>
@@ -1778,34 +1835,35 @@
       <c r="J18" s="7">
         <v>10198.06</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>19</v>
+        <v>107</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D19" s="4">
         <v>10922.0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="H19" s="5">
         <v>0.222</v>
@@ -1816,36 +1874,37 @@
       <c r="J19" s="7">
         <v>107902.7</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>19</v>
+        <v>112</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D20" s="4">
         <v>4238.0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="9">
+        <v>117</v>
+      </c>
+      <c r="H20" s="10">
         <v>0.48</v>
       </c>
       <c r="I20" s="6">
@@ -1854,34 +1913,35 @@
       <c r="J20" s="7">
         <v>67821.87</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>19</v>
+        <v>118</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D21" s="4">
         <v>8217.0</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H21" s="5">
         <v>0.423</v>
@@ -1892,34 +1952,35 @@
       <c r="J21" s="7">
         <v>840911.21</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>19</v>
+        <v>123</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D22" s="4">
         <v>8669.0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H22" s="5">
         <v>0.398</v>
@@ -1930,34 +1991,35 @@
       <c r="J22" s="7">
         <v>77619.21</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>19</v>
+        <v>128</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D23" s="4">
         <v>2694.0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="H23" s="5">
         <v>0.251</v>
@@ -1968,34 +2030,35 @@
       <c r="J23" s="7">
         <v>28167.08</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>128</v>
-      </c>
+      <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>19</v>
+        <v>133</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D24" s="4">
         <v>26490.0</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H24" s="5">
         <v>0.175</v>
@@ -2006,34 +2069,35 @@
       <c r="J24" s="7">
         <v>1889708.19</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>19</v>
+        <v>139</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D25" s="4">
         <v>6465.0</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H25" s="3">
         <v>30.45</v>
@@ -2044,148 +2108,152 @@
       <c r="J25" s="7">
         <v>36740.97</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>19</v>
+        <v>144</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>150</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="I27" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="J27" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="K28" s="3"/>
+      <c r="L28" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>151</v>
+      <c r="M28" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D29" s="4">
         <v>3011.0</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="H29" s="5">
         <v>0.316</v>
@@ -2196,34 +2264,35 @@
       <c r="J29" s="8">
         <v>378262.0</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>161</v>
-      </c>
+      <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>151</v>
+        <v>166</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D30" s="4">
         <v>1001.0</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="H30" s="3">
         <v>47.5</v>
@@ -2234,34 +2303,35 @@
       <c r="J30" s="8">
         <v>21840.0</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>167</v>
-      </c>
+      <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>151</v>
+        <v>172</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D31" s="4">
         <v>308.0</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="H31" s="5">
         <v>0.353</v>
@@ -2272,34 +2342,35 @@
       <c r="J31" s="8">
         <v>30653.0</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>151</v>
+        <v>178</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D32" s="4">
         <v>963.0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H32" s="5">
         <v>0.348</v>
@@ -2310,34 +2381,35 @@
       <c r="J32" s="8">
         <v>6500.0</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>178</v>
-      </c>
+      <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>151</v>
+        <v>183</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D33" s="4">
         <v>8764.0</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="H33" s="5">
         <v>0.228</v>
@@ -2348,34 +2420,35 @@
       <c r="J33" s="8">
         <v>269921.0</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>183</v>
-      </c>
+      <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>151</v>
+        <v>188</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D34" s="4">
         <v>13409.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="H34" s="5">
         <v>0.484</v>
@@ -2386,34 +2459,35 @@
       <c r="J34" s="8">
         <v>1684226.0</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>151</v>
+        <v>193</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D35" s="4">
         <v>2197.0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H35" s="5">
         <v>0.352</v>
@@ -2424,34 +2498,35 @@
       <c r="J35" s="8">
         <v>43961.0</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>193</v>
-      </c>
+      <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>151</v>
+        <v>198</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D36" s="4">
         <v>11712.0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="H36" s="5">
         <v>0.521</v>
@@ -2462,34 +2537,35 @@
       <c r="J36" s="8">
         <v>371823.0</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>198</v>
-      </c>
+      <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>151</v>
+        <v>203</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D37" s="4">
         <v>465.0</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="H37" s="5">
         <v>0.309</v>
@@ -2500,34 +2576,35 @@
       <c r="J37" s="8">
         <v>188077.0</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="K37" s="3"/>
       <c r="L37" s="3" t="s">
-        <v>151</v>
+        <v>208</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D38" s="4">
         <v>7185.0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H38" s="5">
         <v>0.318</v>
@@ -2538,34 +2615,35 @@
       <c r="J38" s="8">
         <v>1621044.0</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>151</v>
+        <v>213</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D39" s="4">
         <v>1335.0</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="H39" s="5">
         <v>0.351</v>
@@ -2576,34 +2654,35 @@
       <c r="J39" s="8">
         <v>992463.0</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>213</v>
-      </c>
+      <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>151</v>
+        <v>218</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D40" s="4">
         <v>3400.0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="H40" s="5">
         <v>0.223</v>
@@ -2614,34 +2693,35 @@
       <c r="J40" s="8">
         <v>301103.0</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>217</v>
-      </c>
+      <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>151</v>
+        <v>222</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D41" s="4">
         <v>1815.0</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="H41" s="5">
         <v>0.204</v>
@@ -2652,34 +2732,35 @@
       <c r="J41" s="8">
         <v>89619.0</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>221</v>
-      </c>
+      <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>151</v>
+        <v>226</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D42" s="4">
         <v>3254.0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="H42" s="5">
         <v>0.217</v>
@@ -2690,34 +2771,35 @@
       <c r="J42" s="8">
         <v>879917.0</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>226</v>
-      </c>
+      <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>151</v>
+        <v>231</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D43" s="4">
         <v>4043.0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="H43" s="5">
         <v>0.362</v>
@@ -2728,34 +2810,35 @@
       <c r="J43" s="8">
         <v>495423.0</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>230</v>
-      </c>
+      <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>151</v>
+        <v>235</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D44" s="4">
         <v>3613.0</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="H44" s="5">
         <v>0.422</v>
@@ -2766,34 +2849,35 @@
       <c r="J44" s="8">
         <v>460769.0</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>234</v>
-      </c>
+      <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>151</v>
+        <v>239</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D45" s="4">
         <v>3316.0</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H45" s="5">
         <v>0.155</v>
@@ -2804,34 +2888,35 @@
       <c r="J45" s="8">
         <v>12004.0</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>151</v>
+        <v>244</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D46" s="4">
         <v>1886.0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="H46" s="5">
         <v>0.207</v>
@@ -2842,34 +2927,35 @@
       <c r="J46" s="8">
         <v>15034.0</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>243</v>
-      </c>
+      <c r="K46" s="3"/>
       <c r="L46" s="3" t="s">
-        <v>151</v>
+        <v>248</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D47" s="4">
         <v>1727.0</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="H47" s="5">
         <v>0.185</v>
@@ -2880,34 +2966,35 @@
       <c r="J47" s="8">
         <v>50681.0</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>248</v>
-      </c>
+      <c r="K47" s="3"/>
       <c r="L47" s="3" t="s">
-        <v>151</v>
+        <v>253</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D48" s="4">
         <v>1611.0</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H48" s="5">
         <v>0.117</v>
@@ -2918,36 +3005,37 @@
       <c r="J48" s="8">
         <v>19094.0</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>151</v>
+        <v>257</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D49" s="4">
         <v>10068.0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="H49" s="9">
+        <v>261</v>
+      </c>
+      <c r="H49" s="10">
         <v>0.51</v>
       </c>
       <c r="I49" s="6">
@@ -2956,34 +3044,35 @@
       <c r="J49" s="8">
         <v>1822074.0</v>
       </c>
-      <c r="K49" s="3" t="s">
-        <v>257</v>
-      </c>
+      <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>151</v>
+        <v>262</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D50" s="4">
         <v>3185.0</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H50" s="5">
         <v>0.303</v>
@@ -2994,34 +3083,35 @@
       <c r="J50" s="8">
         <v>48930.0</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>261</v>
-      </c>
+      <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
-        <v>151</v>
+        <v>266</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D51" s="4">
         <v>1752.0</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H51" s="5">
         <v>0.131</v>
@@ -3032,34 +3122,35 @@
       <c r="J51" s="8">
         <v>28180.0</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>265</v>
-      </c>
+      <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>151</v>
+        <v>270</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D52" s="4">
         <v>2668.0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="I52" s="6">
         <v>2723.0</v>
@@ -3067,34 +3158,35 @@
       <c r="J52" s="8">
         <v>12236.0</v>
       </c>
-      <c r="K52" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="K52" s="3"/>
       <c r="L52" s="3" t="s">
-        <v>151</v>
+        <v>275</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D53" s="4">
         <v>4965.0</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H53" s="5">
         <v>0.268</v>
@@ -3105,34 +3197,35 @@
       <c r="J53" s="8">
         <v>22890.0</v>
       </c>
-      <c r="K53" s="3" t="s">
-        <v>274</v>
-      </c>
+      <c r="K53" s="3"/>
       <c r="L53" s="3" t="s">
-        <v>151</v>
+        <v>279</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D54" s="4">
         <v>621.0</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H54" s="5">
         <v>0.139</v>
@@ -3143,34 +3236,35 @@
       <c r="J54" s="8">
         <v>77035.0</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>278</v>
-      </c>
+      <c r="K54" s="3"/>
       <c r="L54" s="3" t="s">
-        <v>151</v>
+        <v>283</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="D55" s="4">
         <v>11021.0</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="H55" s="5">
         <v>0.235</v>
@@ -3181,36 +3275,37 @@
       <c r="J55" s="8">
         <v>53437.0</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>283</v>
-      </c>
+      <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>151</v>
+        <v>288</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D56" s="4">
         <v>3255.0</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="H56" s="11">
+        <v>292</v>
+      </c>
+      <c r="H56" s="12">
         <v>32.9</v>
       </c>
       <c r="I56" s="6">
@@ -3219,34 +3314,35 @@
       <c r="J56" s="8">
         <v>71676.0</v>
       </c>
-      <c r="K56" s="3" t="s">
-        <v>288</v>
-      </c>
+      <c r="K56" s="3"/>
       <c r="L56" s="3" t="s">
-        <v>151</v>
+        <v>293</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D57" s="4">
         <v>4384.0</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="H57" s="5">
         <v>0.189</v>
@@ -3257,34 +3353,35 @@
       <c r="J57" s="8">
         <v>96106.0</v>
       </c>
-      <c r="K57" s="3" t="s">
-        <v>293</v>
-      </c>
+      <c r="K57" s="3"/>
       <c r="L57" s="3" t="s">
-        <v>151</v>
+        <v>298</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="D58" s="4">
         <v>841.0</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H58" s="5">
         <v>0.192</v>
@@ -3295,34 +3392,35 @@
       <c r="J58" s="8">
         <v>16813.0</v>
       </c>
-      <c r="K58" s="3" t="s">
-        <v>297</v>
-      </c>
+      <c r="K58" s="3"/>
       <c r="L58" s="3" t="s">
-        <v>151</v>
+        <v>302</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D59" s="4">
         <v>10201.0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H59" s="5">
         <v>0.439</v>
@@ -3333,34 +3431,35 @@
       <c r="J59" s="8">
         <v>2846409.0</v>
       </c>
-      <c r="K59" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="K59" s="3"/>
       <c r="L59" s="3" t="s">
-        <v>151</v>
+        <v>307</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D60" s="4">
         <v>192.0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="H60" s="5">
         <v>0.073</v>
@@ -3371,34 +3470,35 @@
       <c r="J60" s="8">
         <v>1403.0</v>
       </c>
-      <c r="K60" s="3" t="s">
-        <v>307</v>
-      </c>
+      <c r="K60" s="3"/>
       <c r="L60" s="3" t="s">
-        <v>151</v>
+        <v>312</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D61" s="4">
         <v>7891.0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H61" s="5">
         <v>0.443</v>
@@ -3409,15 +3509,20 @@
       <c r="J61" s="8">
         <v>463271.0</v>
       </c>
-      <c r="K61" s="3" t="s">
-        <v>312</v>
-      </c>
+      <c r="K61" s="3"/>
       <c r="L61" s="3" t="s">
-        <v>151</v>
+        <v>317</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="K4"/>
+    <hyperlink r:id="rId3" ref="K5"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>